<commit_message>
Half of work is done
</commit_message>
<xml_diff>
--- a/docs/TA.Final.Requirements.MaximCherviakov.xlsx
+++ b/docs/TA.Final.Requirements.MaximCherviakov.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\Practices\TA.FinalPractice.MaximCherviakov\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\Practices\TA.FinalPractice.MaximCherviakov\ta.sm21.maximcherviakov\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3ACD32-174E-4D29-AB80-DFF7714D40AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36ABCA52-62C0-46B3-BE0B-7ED486E8423C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>Формулировка требований</t>
   </si>
@@ -222,15 +222,9 @@
     <t>Успешное создание объекта типа "Country"</t>
   </si>
   <si>
-    <t>Успешное создание объекта типа "Sity"</t>
-  </si>
-  <si>
     <t>Успешное создание объекта типа "Building"</t>
   </si>
   <si>
-    <t>Успешное создание объекта типа "Floor"</t>
-  </si>
-  <si>
     <t>Успешное создание объекта типа "Pay Boxl"</t>
   </si>
   <si>
@@ -273,9 +267,6 @@
     <t>Значение отрибута "Square" объекта "Building" должно быть больше чем 0.</t>
   </si>
   <si>
-    <t>Значение атрибута "Name" объекта "Floor" должно создаваться автоматически с использованием атрибута "Number" и выглядить так: "Floor#N", где N - значение атрибута "Number".</t>
-  </si>
-  <si>
     <t xml:space="preserve">Значение атрибута "Square" объекта "Room" должно быть больше чем 0, но меньше чем значение атрибута "Square" объекта "Floor" </t>
   </si>
   <si>
@@ -345,9 +336,6 @@
     <t>R1.34</t>
   </si>
   <si>
-    <t>R1.35</t>
-  </si>
-  <si>
     <t>TC_34</t>
   </si>
   <si>
@@ -384,10 +372,13 @@
     <t>TC_38</t>
   </si>
   <si>
-    <t>TC_39</t>
-  </si>
-  <si>
     <t>Если пользователь заполнил значения всех полей согласно требованиям выше, в течение 5 секунд после нажатия на кнопку ‘Register’ он должен увидеть сообщение ‘You have successfully registered’.</t>
+  </si>
+  <si>
+    <t>Успешное создание объекта типа "City"</t>
+  </si>
+  <si>
+    <t>Успешное создание объекта типа "Floor". Значение атрибута "Name" объекта "Floor" должно создаваться автоматически с использованием атрибута "Number" и выглядить так: "Floor#N", где N - значение атрибута "Number".</t>
   </si>
 </sst>
 </file>
@@ -790,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -905,7 +896,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>19</v>
@@ -971,7 +962,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>51</v>
@@ -982,7 +973,7 @@
         <v>40</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>52</v>
@@ -993,7 +984,7 @@
         <v>41</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>53</v>
@@ -1004,18 +995,18 @@
         <v>42</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>55</v>
@@ -1026,51 +1017,51 @@
         <v>44</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>75</v>
+      <c r="B23" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>100</v>
+      <c r="B24" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>101</v>
+      <c r="B25" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>60</v>
@@ -1081,7 +1072,7 @@
         <v>49</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>61</v>
@@ -1089,176 +1080,165 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B32" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="B34" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="B35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" s="4" t="s">
+      <c r="B37" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="10"/>
+    </row>
+    <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="C38" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B39" s="4"/>
+      <c r="C39" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="C38" s="10"/>
-    </row>
-    <row r="39" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B37:C37"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Half of work done
</commit_message>
<xml_diff>
--- a/docs/TA.Final.Requirements.MaximCherviakov.xlsx
+++ b/docs/TA.Final.Requirements.MaximCherviakov.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\Practices\TA.FinalPractice.MaximCherviakov\ta.sm21.maximcherviakov\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36ABCA52-62C0-46B3-BE0B-7ED486E8423C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA4925B-6BC3-4A3A-9B04-55DC7BD27C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>Формулировка требований</t>
   </si>
@@ -379,6 +379,18 @@
   </si>
   <si>
     <t>Успешное создание объекта типа "Floor". Значение атрибута "Name" объекта "Floor" должно создаваться автоматически с использованием атрибута "Number" и выглядить так: "Floor#N", где N - значение атрибута "Number".</t>
+  </si>
+  <si>
+    <t>TC_39</t>
+  </si>
+  <si>
+    <t>TC_40</t>
+  </si>
+  <si>
+    <t>R2.5</t>
+  </si>
+  <si>
+    <t>R2.6</t>
   </si>
 </sst>
 </file>
@@ -781,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38:C41"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1235,6 +1247,22 @@
         <v>114</v>
       </c>
     </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:C2"/>

</xml_diff>

<commit_message>
27 test cases are done
</commit_message>
<xml_diff>
--- a/docs/TA.Final.Requirements.MaximCherviakov.xlsx
+++ b/docs/TA.Final.Requirements.MaximCherviakov.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\Practices\TA.FinalPractice.MaximCherviakov\ta.sm21.maximcherviakov\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B77907-8397-48F6-807F-3174DD97212A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE0A3A0-94C7-4009-B9D1-C3931A223F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -225,9 +225,6 @@
     <t>Успешное создание объекта типа "Building"</t>
   </si>
   <si>
-    <t>Успешное создание объекта типа "Pay Boxl"</t>
-  </si>
-  <si>
     <t>Успешное создание объекта типа "ATM"</t>
   </si>
   <si>
@@ -397,6 +394,9 @@
   </si>
   <si>
     <t>TC_42</t>
+  </si>
+  <si>
+    <t>Успешное создание объекта типа "Pay Box"</t>
   </si>
 </sst>
 </file>
@@ -801,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43:C45"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -914,7 +914,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>19</v>
@@ -980,7 +980,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>51</v>
@@ -991,7 +991,7 @@
         <v>40</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>52</v>
@@ -1013,7 +1013,7 @@
         <v>42</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>54</v>
@@ -1024,7 +1024,7 @@
         <v>43</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>55</v>
@@ -1035,7 +1035,7 @@
         <v>44</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>56</v>
@@ -1046,7 +1046,7 @@
         <v>45</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>57</v>
@@ -1057,7 +1057,7 @@
         <v>46</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>58</v>
@@ -1068,7 +1068,7 @@
         <v>47</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>59</v>
@@ -1079,7 +1079,7 @@
         <v>48</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>60</v>
@@ -1090,7 +1090,7 @@
         <v>49</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>61</v>
@@ -1098,185 +1098,185 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C37" s="10"/>
     </row>
     <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="C38" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C44" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C45" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>